<commit_message>
Modified, simplified some activities
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\Student_Grade_Calculation_Robot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83034F6-ECB0-4446-818B-E6BB9BED9CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3613E34-2139-45BD-A648-1081B0427315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="1035" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -113,10 +113,10 @@
     <t>Emanual</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>Average</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -448,12 +448,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1D7BCA-18BE-42CE-91D9-37A4FCBE4D62}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0736076-942C-44C8-8CA5-3A1798067261}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -462,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -586,7 +584,7 @@
         <v>3.6666666666666665</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -598,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="F2:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +878,7 @@
         <v>3.6666666666666701</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Get Color and Set Range Color activities
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\Student_Grade_Calculation_Robot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3613E34-2139-45BD-A648-1081B0427315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B40E400-F875-492B-A0CC-8C5890F61BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1035" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -143,15 +143,51 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -159,16 +195,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,143 +535,148 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0736076-942C-44C8-8CA5-3A1798067261}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>14.333333333333334</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="B2" s="2">
+        <v>19.333333333333332</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>18</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="2">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>14.666666666666666</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>13.333333333333334</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>15.333333333333334</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
         <v>16.666666666666668</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>15.333333333333334</v>
-      </c>
-      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>19.333333333333332</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="2">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9">
-        <v>16.666666666666668</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>14.333333333333334</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>14.666666666666666</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="B11" s="2">
+        <v>13.333333333333334</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>3.6666666666666665</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
+    <sortCondition ref="C2:C12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -596,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="F2:G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,49 +695,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2">
-        <v>18</v>
-      </c>
-      <c r="F2">
-        <v>14.3333333333333</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
+        <v>17</v>
+      </c>
+      <c r="C2" s="7">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7">
+        <v>19</v>
+      </c>
+      <c r="E2" s="7">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2">
+        <v>19.3333333333333</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -658,204 +747,204 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2">
-        <v>18</v>
-      </c>
-      <c r="E3" s="2">
-        <v>18</v>
-      </c>
-      <c r="F3">
-        <v>18</v>
-      </c>
-      <c r="G3">
+      <c r="C3" s="7">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2">
         <v>15</v>
       </c>
-      <c r="E4" s="2">
-        <v>19</v>
-      </c>
-      <c r="F4">
-        <v>14.6666666666667</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
+      <c r="C4" s="7">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7">
+        <v>17</v>
+      </c>
+      <c r="E4" s="7">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2">
+        <v>16.6666666666667</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>13.3333333333333</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
+      <c r="E5" s="7">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2">
+        <v>15.3333333333333</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="7">
+        <v>17</v>
+      </c>
+      <c r="D6" s="7">
         <v>15</v>
       </c>
-      <c r="C6" s="2">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2">
-        <v>18</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="7">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2">
         <v>16.6666666666667</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2">
-        <v>19</v>
-      </c>
-      <c r="F7">
-        <v>15.3333333333333</v>
-      </c>
-      <c r="G7">
+        <v>21</v>
+      </c>
+      <c r="C7" s="7">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="7">
         <v>17</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="7">
+        <v>18</v>
+      </c>
+      <c r="E8" s="7">
         <v>19</v>
       </c>
-      <c r="D8" s="2">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2">
-        <v>20</v>
-      </c>
-      <c r="F8">
-        <v>19.3333333333333</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
+      <c r="F8" s="2">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="2">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="7">
         <v>15</v>
       </c>
-      <c r="E9" s="2">
-        <v>18</v>
-      </c>
-      <c r="F9">
-        <v>16.6666666666667</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
+      <c r="D9" s="7">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7">
+        <v>18</v>
+      </c>
+      <c r="F9" s="2">
+        <v>14.3333333333333</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="2">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2">
+        <v>12</v>
+      </c>
+      <c r="C10" s="7">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7">
         <v>15</v>
       </c>
-      <c r="E10" s="2">
-        <v>18</v>
-      </c>
-      <c r="F10">
-        <v>17</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
+      <c r="E10" s="7">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2">
+        <v>14.6666666666667</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2">
-        <v>17</v>
-      </c>
-      <c r="D11" s="2">
-        <v>18</v>
-      </c>
-      <c r="E11" s="2">
-        <v>19</v>
-      </c>
-      <c r="F11">
-        <v>18</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="C11" s="7">
+        <v>12</v>
+      </c>
+      <c r="D11" s="7">
+        <v>13</v>
+      </c>
+      <c r="E11" s="7">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2">
+        <v>13.3333333333333</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -865,19 +954,19 @@
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="8">
+        <v>2</v>
+      </c>
+      <c r="D12" s="8">
         <v>5</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="8">
         <v>4</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>3.6666666666666701</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -887,6 +976,9 @@
       <c r="E13" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
+    <sortCondition ref="G2:G12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Copy and Delete sheet activities
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\Student_Grade_Calculation_Robot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41157CB3-0689-4FB9-9A22-B28B3F40A373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C591F01-5304-4EEE-BC1A-0BAD5C259013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="CopiedSheet" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -706,7 +707,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A13:XFD20"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72532A2-C3C2-405F-BCE1-579F16A74193}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -1112,4 +1113,276 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D0D904-0EFC-4A07-A959-2FE47D0AB604}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7">
+        <v>19</v>
+      </c>
+      <c r="E2" s="7">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2">
+        <v>19.3333333333333</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7">
+        <v>17</v>
+      </c>
+      <c r="E4" s="7">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2">
+        <v>16.6666666666667</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7">
+        <v>13</v>
+      </c>
+      <c r="E5" s="7">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2">
+        <v>15.3333333333333</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="7">
+        <v>17</v>
+      </c>
+      <c r="D6" s="7">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2">
+        <v>16.6666666666667</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="7">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="7">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7">
+        <v>18</v>
+      </c>
+      <c r="E8" s="7">
+        <v>19</v>
+      </c>
+      <c r="F8" s="2">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="7">
+        <v>15</v>
+      </c>
+      <c r="D9" s="7">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7">
+        <v>18</v>
+      </c>
+      <c r="F9" s="2">
+        <v>14.3333333333333</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="7">
+        <v>12</v>
+      </c>
+      <c r="D10" s="7">
+        <v>13</v>
+      </c>
+      <c r="E10" s="7">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2">
+        <v>13.3333333333333</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>5</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3.6666666666666701</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>